<commit_message>
Major updates in members and added link to directory map
</commit_message>
<xml_diff>
--- a/public/directory/members.xlsx
+++ b/public/directory/members.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="580" windowWidth="25360" windowHeight="15380" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="580" windowWidth="25380" windowHeight="15380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="members" sheetId="1" r:id="rId1"/>
@@ -380,8 +380,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -393,10 +399,16 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="10">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -728,8 +740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="W13" sqref="W13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>

</xml_diff>